<commit_message>
connected the lines and added t-test p values
</commit_message>
<xml_diff>
--- a/MD_simulations/Distances between Asp-Asn Asp-Arg/Asp_Asn_Arg_distances.xlsx
+++ b/MD_simulations/Distances between Asp-Asn Asp-Arg/Asp_Asn_Arg_distances.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eawag\userdata\felderfl\My Documents\GitHub\biodefluorination\modeling\alphafold_models\Distances of residues in structures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eawag\userdata\felderfl\My Documents\GitHub\gut_microbe_defluorination_paper\MD_simulations\Distances between Asp-Asn Asp-Arg\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,16 +15,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$B$11:$B$21</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$B$6:$B$10</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$11:$B$21</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$6:$B$10</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$11:$C$21</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$6:$C$10</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$B$11:$B$21</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$B$6:$B$10</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$11:$B$21</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$6:$B$10</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$10:$C$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$5:$C$9</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$B$10:$B$20</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$B$5:$B$9</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>Distances in Angström (0.1 nm)</t>
   </si>
@@ -80,9 +74,6 @@
     <t>PA0810</t>
   </si>
   <si>
-    <t>WP1187090781 (P1)</t>
-  </si>
-  <si>
     <t>GKG91607 (P2)</t>
   </si>
   <si>
@@ -123,6 +114,12 @@
   </si>
   <si>
     <t>Defluorinating n=11</t>
+  </si>
+  <si>
+    <t>Two sided t-test assuming equal variance</t>
+  </si>
+  <si>
+    <t>p-value</t>
   </si>
 </sst>
 </file>
@@ -208,12 +205,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.4</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -239,6 +236,32 @@
               <a:rPr lang="de-DE" sz="2000" baseline="0"/>
               <a:t>Arg(Nɳ2)</a:t>
             </a:r>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-DE" sz="2000" baseline="0"/>
+              <a:t> p-value = </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-CH" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>0.24</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t>  </a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="2000" baseline="0"/>
           </a:p>
         </cx:rich>
       </cx:tx>
@@ -346,12 +369,12 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -385,6 +408,42 @@
               <a:rPr lang="de-DE" sz="2000" baseline="0"/>
               <a:t>)</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr sz="2000" baseline="0"/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>p-value = </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-CH" sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+              </a:rPr>
+              <a:t>0.19</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-CH"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:endParaRPr lang="de-DE" sz="2000" baseline="0"/>
           </a:p>
         </cx:rich>
       </cx:tx>
@@ -1549,7 +1608,7 @@
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>9072</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>54429</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1611,13 +1670,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>239940</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>120196</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>596901</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>34471</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -1679,8 +1738,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E21" totalsRowShown="0">
-  <autoFilter ref="A3:E21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E20" totalsRowShown="0">
+  <autoFilter ref="A3:E20"/>
   <sortState ref="A4:E21">
     <sortCondition ref="E3:E21"/>
   </sortState>
@@ -1958,10 +2017,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1980,24 +2039,24 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>27</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4">
         <v>6.3310000000000004</v>
@@ -2014,16 +2073,16 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5">
-        <v>6.5410000000000004</v>
+        <v>6.6379999999999999</v>
       </c>
       <c r="C5">
-        <v>6.1379999999999999</v>
+        <v>6.2439999999999998</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -2031,13 +2090,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>6.6379999999999999</v>
+        <v>6.1920000000000002</v>
       </c>
       <c r="C6">
-        <v>6.2439999999999998</v>
+        <v>6.1230000000000002</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -2048,13 +2107,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>6.1920000000000002</v>
+        <v>6.4029999999999996</v>
       </c>
       <c r="C7">
-        <v>6.1230000000000002</v>
+        <v>5.8369999999999997</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -2065,13 +2124,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8">
-        <v>6.4029999999999996</v>
+        <v>6.38</v>
       </c>
       <c r="C8">
-        <v>5.8369999999999997</v>
+        <v>6.2789999999999999</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -2082,13 +2141,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9">
-        <v>6.38</v>
+        <v>6.52</v>
       </c>
       <c r="C9">
-        <v>6.2789999999999999</v>
+        <v>6.8010000000000002</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -2099,30 +2158,30 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B10">
-        <v>6.52</v>
+        <v>6.7130000000000001</v>
       </c>
       <c r="C10">
-        <v>6.8010000000000002</v>
+        <v>6.3</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11">
-        <v>6.7130000000000001</v>
+        <v>6.8869999999999996</v>
       </c>
       <c r="C11">
-        <v>6.3</v>
+        <v>6.4960000000000004</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -2133,13 +2192,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="B12">
-        <v>6.8869999999999996</v>
+        <v>6.5469999999999997</v>
       </c>
       <c r="C12">
-        <v>6.4960000000000004</v>
+        <v>5.92</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -2150,13 +2209,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>6.5469999999999997</v>
+        <v>6.6</v>
       </c>
       <c r="C13">
-        <v>5.92</v>
+        <v>6.5259999999999998</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -2167,13 +2226,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>6.6</v>
+        <v>6.5430000000000001</v>
       </c>
       <c r="C14">
-        <v>6.5259999999999998</v>
+        <v>6.1040000000000001</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -2184,13 +2243,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B15">
-        <v>6.5430000000000001</v>
+        <v>6.67</v>
       </c>
       <c r="C15">
-        <v>6.1040000000000001</v>
+        <v>6.0839999999999996</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -2201,13 +2260,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B16">
-        <v>6.67</v>
+        <v>6.4240000000000004</v>
       </c>
       <c r="C16">
-        <v>6.0839999999999996</v>
+        <v>6.4260000000000002</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -2218,13 +2277,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>6.4240000000000004</v>
+        <v>6.2460000000000004</v>
       </c>
       <c r="C17">
-        <v>6.4260000000000002</v>
+        <v>6.91</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -2235,13 +2294,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>6.2460000000000004</v>
+        <v>6.3040000000000003</v>
       </c>
       <c r="C18">
-        <v>6.91</v>
+        <v>5.827</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -2252,13 +2311,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B19">
-        <v>6.3040000000000003</v>
+        <v>6.3879999999999999</v>
       </c>
       <c r="C19">
-        <v>5.827</v>
+        <v>5.8520000000000003</v>
       </c>
       <c r="D19">
         <v>1</v>
@@ -2269,13 +2328,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B20">
-        <v>6.3879999999999999</v>
+        <v>6.5430000000000001</v>
       </c>
       <c r="C20">
-        <v>5.8520000000000003</v>
+        <v>6.1310000000000002</v>
       </c>
       <c r="D20">
         <v>1</v>
@@ -2286,58 +2345,67 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>15</v>
-      </c>
-      <c r="B21">
-        <v>6.5430000000000001</v>
-      </c>
-      <c r="C21">
-        <v>6.1310000000000002</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
         <v>5</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>25</v>
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <f>AVERAGE(B10:B20)</f>
+        <v>6.5331818181818191</v>
+      </c>
+      <c r="C24">
+        <f>AVERAGE(C10:C20)</f>
+        <v>6.2341818181818187</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <f>AVERAGE(B11:B21)</f>
-        <v>6.5331818181818191</v>
+        <f>AVERAGE(B5:B9)</f>
+        <v>6.4265999999999988</v>
       </c>
       <c r="C25">
-        <f>AVERAGE(C11:C21)</f>
-        <v>6.2341818181818187</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26">
-        <f>AVERAGE(B6:B10)</f>
-        <v>6.4265999999999988</v>
-      </c>
-      <c r="C26">
-        <f>AVERAGE(C6:C10)</f>
+        <f>AVERAGE(C5:C9)</f>
         <v>6.2568000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f>_xlfn.T.TEST(B4:B9,B10:B20,2,2)</f>
+        <v>0.19181549369619025</v>
+      </c>
+      <c r="C30">
+        <f>_xlfn.T.TEST(C4:C9,C10:C20,2,2)</f>
+        <v>0.2433713356358187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>